<commit_message>
added the files of the previous year
</commit_message>
<xml_diff>
--- a/I1/DevilerablesAndRoles2.xlsx
+++ b/I1/DevilerablesAndRoles2.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Документи" sheetId="1" r:id="rId1"/>
     <sheet name="Роли" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="99">
   <si>
     <t> Наименование</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>rup_prggd.dot</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>2|4</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -594,6 +600,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -901,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M57"/>
+  <dimension ref="A2:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,13 +925,13 @@
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
     <col min="3" max="7" width="7.7109375" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="25" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="9" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10" style="16" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="25" customWidth="1"/>
+    <col min="14" max="14" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -948,8 +960,9 @@
       <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" s="30"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>1</v>
       </c>
@@ -980,14 +993,17 @@
       <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="30">
+        <v>1</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="M3" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2</v>
       </c>
@@ -1018,14 +1034,17 @@
       <c r="J4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="30">
+        <v>3</v>
+      </c>
+      <c r="L4" s="18">
         <v>2</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="M4" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>3</v>
       </c>
@@ -1056,11 +1075,14 @@
       <c r="J5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="30">
+        <v>5</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>4</v>
       </c>
@@ -1089,14 +1111,15 @@
       <c r="J6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="30"/>
+      <c r="L6" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="M6" s="25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>5</v>
       </c>
@@ -1127,14 +1150,17 @@
       <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="30">
         <v>5</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="18">
+        <v>5</v>
+      </c>
+      <c r="M7" s="26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>6</v>
       </c>
@@ -1151,14 +1177,17 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="18">
+      <c r="K8" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="18">
         <v>3</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="M8" s="26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>7</v>
       </c>
@@ -1189,11 +1218,14 @@
       <c r="J9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>8</v>
       </c>
@@ -1220,11 +1252,12 @@
       <c r="J10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="30"/>
+      <c r="L10" s="19">
         <v>3.4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>9</v>
       </c>
@@ -1255,14 +1288,17 @@
       <c r="J11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="M11" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>10</v>
       </c>
@@ -1281,14 +1317,17 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="30">
+        <v>4</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="M12" s="26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>11</v>
       </c>
@@ -1315,11 +1354,12 @@
       <c r="J13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="30"/>
+      <c r="L13" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>12</v>
       </c>
@@ -1350,11 +1390,12 @@
       <c r="J14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="30"/>
+      <c r="L14" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>13</v>
       </c>
@@ -1385,14 +1426,15 @@
       <c r="J15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="30"/>
+      <c r="L15" s="19">
         <v>4</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="M15" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>14</v>
       </c>
@@ -1417,11 +1459,12 @@
       <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="30"/>
+      <c r="L16" s="19">
         <v>3.4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>15</v>
       </c>
@@ -1448,14 +1491,15 @@
       <c r="J17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="30"/>
+      <c r="L17" s="19">
         <v>1.2</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="M17" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>16</v>
       </c>
@@ -1478,14 +1522,15 @@
       <c r="J18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="30"/>
+      <c r="L18" s="19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="M18" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>17</v>
       </c>
@@ -1510,11 +1555,12 @@
       <c r="J19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="30"/>
+      <c r="L19" s="19">
         <v>3.4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>18</v>
       </c>
@@ -1533,11 +1579,12 @@
       <c r="J20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="30"/>
+      <c r="L20" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>19</v>
       </c>
@@ -1564,14 +1611,15 @@
       <c r="J21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="30"/>
+      <c r="L21" s="19">
         <v>2</v>
       </c>
-      <c r="L21" s="25" t="s">
+      <c r="M21" s="25" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>20</v>
       </c>
@@ -1598,11 +1646,12 @@
         <v>8</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="19">
+      <c r="K22" s="30"/>
+      <c r="L22" s="19">
         <v>2.4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>21</v>
       </c>
@@ -1625,11 +1674,12 @@
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="19">
+      <c r="K23" s="30"/>
+      <c r="L23" s="19">
         <v>2.4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>22</v>
       </c>
@@ -1652,14 +1702,15 @@
       <c r="J24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="30"/>
+      <c r="L24" s="19">
         <v>5</v>
       </c>
-      <c r="L24" s="25" t="s">
+      <c r="M24" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>23</v>
       </c>
@@ -1682,11 +1733,12 @@
       <c r="J25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="30"/>
+      <c r="L25" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>24</v>
       </c>
@@ -1711,11 +1763,12 @@
       <c r="J26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="30"/>
+      <c r="L26" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>25</v>
       </c>
@@ -1736,185 +1789,186 @@
         <v>13</v>
       </c>
       <c r="J27" s="5"/>
-      <c r="K27" s="19">
+      <c r="K27" s="30"/>
+      <c r="L27" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
-      <c r="K28" s="19"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L31" s="28" t="s">
+      <c r="L28" s="19"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M31" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M31" s="29"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K32" s="8"/>
-      <c r="L32" s="21" t="s">
+      <c r="N31" s="29"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L32" s="8"/>
+      <c r="M32" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="N32" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="11:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="K33" s="8"/>
-      <c r="L33" s="20" t="s">
+    <row r="33" spans="12:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="L33" s="8"/>
+      <c r="M33" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M33" s="23" t="s">
+      <c r="N33" s="23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K34" s="8"/>
-      <c r="L34" s="20" t="s">
+    <row r="34" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="8"/>
+      <c r="M34" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M34" s="24" t="s">
+      <c r="N34" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="11:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="K35" s="8"/>
-      <c r="L35" s="20" t="s">
+    <row r="35" spans="12:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="L35" s="8"/>
+      <c r="M35" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M35" s="23" t="s">
+      <c r="N35" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K36" s="8"/>
-      <c r="L36" s="20" t="s">
+    <row r="36" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L36" s="8"/>
+      <c r="M36" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M36" s="23" t="s">
+      <c r="N36" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K37" s="8"/>
-      <c r="L37" s="28" t="s">
+    <row r="37" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L37" s="8"/>
+      <c r="M37" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="M37" s="29"/>
-    </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K38" s="8"/>
-      <c r="L38" s="21" t="s">
+      <c r="N37" s="29"/>
+    </row>
+    <row r="38" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L38" s="8"/>
+      <c r="M38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M38" s="22" t="s">
+      <c r="N38" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K39" s="8"/>
-      <c r="L39" s="20" t="s">
+    <row r="39" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L39" s="8"/>
+      <c r="M39" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="M39" s="24" t="s">
+      <c r="N39" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K40" s="8"/>
-      <c r="L40" s="20" t="s">
+    <row r="40" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L40" s="8"/>
+      <c r="M40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="M40" s="24" t="s">
+      <c r="N40" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K41" s="8"/>
-      <c r="L41" s="20" t="s">
+    <row r="41" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L41" s="8"/>
+      <c r="M41" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="M41" s="24" t="s">
+      <c r="N41" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K42" s="8"/>
-      <c r="L42" s="20" t="s">
+    <row r="42" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L42" s="8"/>
+      <c r="M42" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="M42" s="24" t="s">
+      <c r="N42" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K43" s="8"/>
-    </row>
-    <row r="44" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K44" s="8"/>
-      <c r="M44" s="6"/>
-    </row>
-    <row r="45" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K45" s="8"/>
-      <c r="M45" s="6"/>
-    </row>
-    <row r="46" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K46" s="8"/>
-      <c r="M46" s="6"/>
-    </row>
-    <row r="47" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K47" s="8"/>
-      <c r="M47" s="6"/>
-    </row>
-    <row r="48" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K48" s="8"/>
-      <c r="M48" s="6"/>
-    </row>
-    <row r="49" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K49" s="8"/>
-      <c r="M49" s="6"/>
-    </row>
-    <row r="50" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K50" s="8"/>
-      <c r="M50" s="7"/>
-    </row>
-    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K51" s="8"/>
-      <c r="M51" s="7"/>
-    </row>
-    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K52" s="8"/>
-      <c r="M52" s="6"/>
-    </row>
-    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K53" s="8"/>
-      <c r="M53" s="6"/>
-    </row>
-    <row r="54" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K54" s="8"/>
-      <c r="M54" s="6"/>
-    </row>
-    <row r="55" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K55" s="8"/>
-      <c r="M55" s="6"/>
-    </row>
-    <row r="56" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K56" s="8"/>
-      <c r="M56" s="6"/>
-    </row>
-    <row r="57" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K57" s="8"/>
-      <c r="M57" s="6"/>
+    <row r="43" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L44" s="8"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L45" s="8"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L46" s="8"/>
+      <c r="N46" s="6"/>
+    </row>
+    <row r="47" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L47" s="8"/>
+      <c r="N47" s="6"/>
+    </row>
+    <row r="48" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L48" s="8"/>
+      <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L49" s="8"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L50" s="8"/>
+      <c r="N50" s="7"/>
+    </row>
+    <row r="51" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L51" s="8"/>
+      <c r="N51" s="7"/>
+    </row>
+    <row r="52" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L52" s="8"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L53" s="8"/>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L54" s="8"/>
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L55" s="8"/>
+      <c r="N55" s="6"/>
+    </row>
+    <row r="56" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L56" s="8"/>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="57" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L57" s="8"/>
+      <c r="N57" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M37:N37"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L8" r:id="rId1" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/req/rup_vision_sp.dot"/>
-    <hyperlink ref="L7" r:id="rId2" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/req/rup_gloss.dot"/>
-    <hyperlink ref="L12" r:id="rId3" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/environ/rup_prggd.dot"/>
+    <hyperlink ref="M8" r:id="rId1" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/req/rup_vision_sp.dot"/>
+    <hyperlink ref="M7" r:id="rId2" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/req/rup_gloss.dot"/>
+    <hyperlink ref="M12" r:id="rId3" display="http://sce.uhcl.edu/helm/rationalunifiedprocess/wordtmpl/DOT/environ/rup_prggd.dot"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1925,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>